<commit_message>
Added country language to speech
</commit_message>
<xml_diff>
--- a/src/main/resources/Employees.xlsx
+++ b/src/main/resources/Employees.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atmak\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atmak\IdeaProjects\cheetah-server\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD80147F-45A4-4C85-9CCE-318CBDBC1EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC215B6-F5EB-4E17-B56F-B13D6B670AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>Sandhya</t>
   </si>
@@ -61,6 +61,21 @@
   </si>
   <si>
     <t>Vimal Chandra</t>
+  </si>
+  <si>
+    <t>countryLang</t>
+  </si>
+  <si>
+    <t>te-IN</t>
+  </si>
+  <si>
+    <t>en-IN</t>
+  </si>
+  <si>
+    <t>en-KE</t>
+  </si>
+  <si>
+    <t>kn-IN</t>
   </si>
 </sst>
 </file>
@@ -387,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -401,7 +416,7 @@
     <col min="5" max="5" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -417,8 +432,11 @@
       <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2534678</v>
       </c>
@@ -434,8 +452,11 @@
       <c r="E2" t="s">
         <v>2</v>
       </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>4537821</v>
       </c>
@@ -451,8 +472,11 @@
       <c r="E3" t="s">
         <v>2</v>
       </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2234868</v>
       </c>
@@ -468,8 +492,11 @@
       <c r="E4" t="s">
         <v>2</v>
       </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2564829</v>
       </c>
@@ -484,6 +511,9 @@
       </c>
       <c r="E5" t="s">
         <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>